<commit_message>
Importer should be working now
</commit_message>
<xml_diff>
--- a/dr2/data/content_script/content.xlsx
+++ b/dr2/data/content_script/content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jvargas/Documents/GitHub/datamapper/dr2/data/content_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333DD4B2-8116-8940-8B88-07EA3948CD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBBBC22-3A2E-824D-8D65-F5093A18839D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="880" windowWidth="29740" windowHeight="17860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="880" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="proms" sheetId="1" r:id="rId1"/>
@@ -717,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A12" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1302,7 +1302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GUI app for importer
</commit_message>
<xml_diff>
--- a/dr2/data/content_script/content.xlsx
+++ b/dr2/data/content_script/content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jvargas/Documents/GitHub/datamapper/dr2/data/content_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBBBC22-3A2E-824D-8D65-F5093A18839D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECBDEDD-F3AF-1E4B-852A-C4F1BE98B19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="880" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -275,9 +275,6 @@
     <t xml:space="preserve">&lt;b&gt;Empower cases to create limits&lt;/b&gt; &lt;br&gt; &lt;br&gt; &lt;b&gt; descrption&lt;/b&gt; </t>
   </si>
   <si>
-    <t>&lt;b&gt; Sence &lt;/b&gt; &lt;br&gt; &lt;br&gt; Using senses as a tool for understanding cities involves immersing ourselves in their sensory experiences. By engaging with the sights, sounds, and even the tactile sensations of urban environments, we can discern their unique rhythms, cultures, and dynamics. This sensory-driven approach deepens our connection to cities, unveiling layers of meaning that go beyond conventional analyses. &lt;img src='data/img1.jpg' width='100%' height='auto'&gt; &lt;/img&gt;</t>
-  </si>
-  <si>
     <t>&lt;b&gt; Lifeworlds &lt;/b&gt; &lt;br&gt; &lt;br&gt; Lifeworld refers to the subjective and experiential reality of individuals within their immediate living environment. In the context of livable spaces, lifeworld encompasses the personal perceptions, emotions, and interactions that individuals have with their surroundings. It includes how people interpret and make sense of their environment, the routines and rituals they engage in, and the emotional connections they develop with the spaces they inhabit. Understanding lifeworld is crucial for creating truly livable spaces that cater to the holistic needs and well-being of the people who inhabit them.</t>
   </si>
   <si>
@@ -348,6 +345,9 @@
   </si>
   <si>
     <t>&lt;a href='https://ur-scape.sec.sg/en/home' target='_blank'&gt; ur-scape &lt;/a&gt; is an open-source planning support tool specifically designed to assist towns, cities and regions experiencing rapid urbanisation. It addresses urgent and complex challenges that arise in such areas by harnessing the available geospatial data however diverse and varied in quality. By seamlessly combining different types, scales and sources of those data, ur-scape provides intuitive, interactive and reliable outputs that can be easily navigated and analysed in real-time.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt; Sense &lt;/b&gt; &lt;br&gt; &lt;br&gt; Using senses as a tool for understanding cities involves immersing ourselves in their sensory experiences. By engaging with the sights, sounds, and even the tactile sensations of urban environments, we can discern their unique rhythms, cultures, and dynamics. This sensory-driven approach deepens our connection to cities, unveiling layers of meaning that go beyond conventional analyses. &lt;img src='data/img1.jpg' width='100%' height='auto'&gt; &lt;/img&gt;</t>
   </si>
 </sst>
 </file>
@@ -1302,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1456,7 +1456,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1467,7 +1467,7 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1478,7 +1478,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1489,7 +1489,7 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1500,7 +1500,7 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1511,7 +1511,7 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1522,7 +1522,7 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1533,7 +1533,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1544,7 +1544,7 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1555,7 +1555,7 @@
         <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1566,7 +1566,7 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1577,7 +1577,7 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1588,7 +1588,7 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1599,7 +1599,7 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1610,7 +1610,7 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1621,7 +1621,7 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1632,7 +1632,7 @@
         <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1643,7 +1643,7 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1654,7 +1654,7 @@
         <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1665,7 +1665,7 @@
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1676,7 +1676,7 @@
         <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1687,7 +1687,7 @@
         <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1698,7 +1698,7 @@
         <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1709,7 +1709,7 @@
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1720,7 +1720,7 @@
         <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expand Excel Converter into full Data Import app
</commit_message>
<xml_diff>
--- a/dr2/data/content_script/content.xlsx
+++ b/dr2/data/content_script/content.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jvargas/Documents/GitHub/datamapper/dr2/data/content_script/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECBDEDD-F3AF-1E4B-852A-C4F1BE98B19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="880" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="proms" sheetId="1" r:id="rId1"/>
     <sheet name="description" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -275,6 +269,9 @@
     <t xml:space="preserve">&lt;b&gt;Empower cases to create limits&lt;/b&gt; &lt;br&gt; &lt;br&gt; &lt;b&gt; descrption&lt;/b&gt; </t>
   </si>
   <si>
+    <t>&lt;b&gt; Sense &lt;/b&gt; &lt;br&gt; &lt;br&gt; Using senses as a tool for understanding cities involves immersing ourselves in their sensory experiences. By engaging with the sights, sounds, and even the tactile sensations of urban environments, we can discern their unique rhythms, cultures, and dynamics. This sensory-driven approach deepens our connection to cities, unveiling layers of meaning that go beyond conventional analyses. &lt;img src='data/img1.jpg' width='100%' height='auto'&gt; &lt;/img&gt;</t>
+  </si>
+  <si>
     <t>&lt;b&gt; Lifeworlds &lt;/b&gt; &lt;br&gt; &lt;br&gt; Lifeworld refers to the subjective and experiential reality of individuals within their immediate living environment. In the context of livable spaces, lifeworld encompasses the personal perceptions, emotions, and interactions that individuals have with their surroundings. It includes how people interpret and make sense of their environment, the routines and rituals they engage in, and the emotional connections they develop with the spaces they inhabit. Understanding lifeworld is crucial for creating truly livable spaces that cater to the holistic needs and well-being of the people who inhabit them.</t>
   </si>
   <si>
@@ -345,16 +342,13 @@
   </si>
   <si>
     <t>&lt;a href='https://ur-scape.sec.sg/en/home' target='_blank'&gt; ur-scape &lt;/a&gt; is an open-source planning support tool specifically designed to assist towns, cities and regions experiencing rapid urbanisation. It addresses urgent and complex challenges that arise in such areas by harnessing the available geospatial data however diverse and varied in quality. By seamlessly combining different types, scales and sources of those data, ur-scape provides intuitive, interactive and reliable outputs that can be easily navigated and analysed in real-time.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt; Sense &lt;/b&gt; &lt;br&gt; &lt;br&gt; Using senses as a tool for understanding cities involves immersing ourselves in their sensory experiences. By engaging with the sights, sounds, and even the tactile sensations of urban environments, we can discern their unique rhythms, cultures, and dynamics. This sensory-driven approach deepens our connection to cities, unveiling layers of meaning that go beyond conventional analyses. &lt;img src='data/img1.jpg' width='100%' height='auto'&gt; &lt;/img&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,21 +411,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -469,7 +455,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -503,7 +489,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -538,10 +523,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -714,14 +698,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,7 +725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -764,7 +748,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -787,7 +771,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -810,7 +794,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -833,7 +817,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -856,7 +840,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -879,7 +863,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -902,7 +886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -925,7 +909,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -948,7 +932,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -971,7 +955,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -994,7 +978,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1017,7 +1001,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1040,7 +1024,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1063,7 +1047,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1086,7 +1070,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1109,7 +1093,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1132,7 +1116,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1155,7 +1139,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1178,7 +1162,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1201,7 +1185,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1224,7 +1208,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1247,7 +1231,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1270,7 +1254,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1299,16 +1283,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1316,7 +1298,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1327,7 +1309,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1338,7 +1320,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1349,7 +1331,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1360,7 +1342,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1371,7 +1353,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1382,7 +1364,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1393,7 +1375,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1404,7 +1386,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1415,7 +1397,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1426,7 +1408,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1437,7 +1419,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1448,7 +1430,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1456,10 +1438,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1467,10 +1449,10 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1478,10 +1460,10 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1489,10 +1471,10 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1500,10 +1482,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1511,10 +1493,10 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1522,10 +1504,10 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1533,10 +1515,10 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1544,10 +1526,10 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1555,10 +1537,10 @@
         <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1566,10 +1548,10 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1577,10 +1559,10 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1588,10 +1570,10 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1599,10 +1581,10 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1610,10 +1592,10 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1621,10 +1603,10 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1632,10 +1614,10 @@
         <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1643,10 +1625,10 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1654,10 +1636,10 @@
         <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1665,10 +1647,10 @@
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1676,10 +1658,10 @@
         <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1687,10 +1669,10 @@
         <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1698,10 +1680,10 @@
         <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1709,10 +1691,10 @@
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1720,7 +1702,7 @@
         <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>